<commit_message>
add test cases for 1.1 in excel file
</commit_message>
<xml_diff>
--- a/doc/Model/Acceptance tests.xlsx
+++ b/doc/Model/Acceptance tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royash/Documents/Workshop-On-Software-Engineering-Project-2019/Documents/Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\sadna\Workshop-On-Software-Engineering-Project-2019\doc\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDB4537-344A-934C-81F8-29AE060A4943}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF89BF0-6FD7-4845-9E69-A444823816DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{1CA65076-1370-4905-AE0F-4695E8F49515}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CA65076-1370-4905-AE0F-4695E8F49515}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
   <si>
     <t>data</t>
   </si>
@@ -260,9 +260,6 @@
     <t>המערכת מחזירה הודעת שגיאה על כך אחד פרטי המשתמש שגויים</t>
   </si>
   <si>
-    <t>המשתמש מחפש מוצר לפי מספר המוצר והמוצר קיים המערכת</t>
-  </si>
-  <si>
     <t>המוצר אותו הזין המשתמש נמצא בתוצאות החיפוש</t>
   </si>
   <si>
@@ -372,6 +369,21 @@
   </si>
   <si>
     <t>המערכת מציגה למשתמש הודעה על כך שהצליח להירשם בהצלחה והמשתמש מוגדר כמנוי במערכת, אך אינו מחובר</t>
+  </si>
+  <si>
+    <t>המערכת אותחלה בהצלחה, קושרה למערכות החיצוניות (עקיבות, גבייה, אספקה) ומונה מנהל מערכת יחיד.</t>
+  </si>
+  <si>
+    <t>מזינים שם משתמש וסיסמה תקינים של מנהל המערכת</t>
+  </si>
+  <si>
+    <t>מזינים שם משתמש וסיסמה לא תקינה של מנהל המערכת</t>
+  </si>
+  <si>
+    <t>המערכת לא אותחלה והוצגה הודעת שגיאה</t>
+  </si>
+  <si>
+    <t>המשתמש מחפש מוצר לפי שם המוצר והמוצר קיים המערכת</t>
   </si>
 </sst>
 </file>
@@ -382,14 +394,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -465,8 +477,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6CFC1F84-449F-47ED-BBEA-4EF5BEC0A93A}" name="Table1" displayName="Table1" ref="B1:E57" totalsRowShown="0" dataDxfId="4">
-  <autoFilter ref="B1:E57" xr:uid="{AD44D35B-AAB7-4FAB-8348-524CACD0E48F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6CFC1F84-449F-47ED-BBEA-4EF5BEC0A93A}" name="Table1" displayName="Table1" ref="B1:E58" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="B1:E58" xr:uid="{AD44D35B-AAB7-4FAB-8348-524CACD0E48F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A7C70BDA-E6BF-4FDC-92ED-77951EB0BE2A}" name="expected result" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{0AF91C84-E078-467D-8BAA-5AAC4C6F1F02}" name="data" dataDxfId="2"/>
@@ -478,7 +490,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -774,23 +786,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB44C02-4CA2-465F-A9FE-5F1D45ACF731}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="42.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.33203125" customWidth="1"/>
-    <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="1" max="1" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.36328125" customWidth="1"/>
+    <col min="3" max="3" width="47.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.36328125" customWidth="1"/>
+    <col min="6" max="6" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -804,789 +816,809 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
       <c r="E2" s="3">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.15">
-      <c r="B3" s="1" t="s">
-        <v>113</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B3" s="3" t="s">
+        <v>116</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
       <c r="D3" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="3">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.15">
-      <c r="B4" s="3" t="s">
-        <v>72</v>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="D4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D5" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="3">
+        <v>3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.15">
-      <c r="B7" s="3" t="s">
-        <v>75</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="D7" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>75</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D8" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" s="3">
+        <v>3</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="3">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.15">
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="D10" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3">
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>94</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E11" s="3">
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="D12" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3">
         <v>2.5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.15">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
+    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D13" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="3">
         <v>2.5</v>
       </c>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.15">
-      <c r="A14" s="2"/>
+    </row>
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="B14" s="3" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="D14" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="3">
         <v>2.5</v>
       </c>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="D15" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="3">
         <v>2.5</v>
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
       <c r="B16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="3">
-        <v>1</v>
-      </c>
-      <c r="E16" s="3">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="60" x14ac:dyDescent="0.15">
-      <c r="B17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D17" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3">
         <v>2.6</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="45" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:5" ht="58" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="3">
         <v>2.6</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="45" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" s="3">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B20" s="3" t="s">
-        <v>97</v>
-      </c>
       <c r="C20" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D20" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="3">
         <v>2.7</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="3">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="3">
-        <v>1</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B22" s="3" t="s">
+    <row r="23" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="3">
-        <v>2</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="D23" s="3">
+        <v>2</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="B23" s="3" t="s">
+    <row r="24" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="3">
-        <v>1</v>
-      </c>
-      <c r="E23" s="3" t="s">
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="B24" s="3" t="s">
+    <row r="25" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="3">
-        <v>2</v>
-      </c>
-      <c r="E24" s="4" t="s">
+      <c r="D25" s="3">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="B25" s="3" t="s">
+    <row r="26" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="3">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3" t="s">
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="B26" s="3" t="s">
+    <row r="27" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="3">
-        <v>2</v>
-      </c>
-      <c r="E26" s="4" t="s">
+      <c r="D27" s="3">
+        <v>2</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="15" x14ac:dyDescent="0.15">
-      <c r="B27" s="1" t="s">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="3">
-        <v>1</v>
-      </c>
-      <c r="E27" s="3">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="15" x14ac:dyDescent="0.15">
-      <c r="B28" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="D28" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="3">
         <v>3.1</v>
       </c>
     </row>
-    <row r="29" spans="2:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="B29" s="1" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="3">
-        <v>1</v>
-      </c>
-      <c r="E29" s="3">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B30" s="1" t="s">
-        <v>99</v>
-      </c>
       <c r="C30" s="3" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="D30" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30" s="3">
         <v>3.2</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>101</v>
+        <v>36</v>
       </c>
       <c r="D31" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" s="3">
         <v>3.2</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="3">
+        <v>3</v>
+      </c>
+      <c r="E32" s="3">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B33" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C33" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="3">
-        <v>1</v>
-      </c>
-      <c r="E32" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B33" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D33" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="3">
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="B34" s="1" t="s">
+    <row r="34" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B34" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="3">
+        <v>2</v>
+      </c>
+      <c r="E34" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B35" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="3">
-        <v>1</v>
-      </c>
-      <c r="E34" s="3">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B35" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D35" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="3">
         <v>4.3</v>
       </c>
     </row>
-    <row r="36" spans="2:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="D36" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E36" s="3">
         <v>4.3</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="D37" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E37" s="3">
         <v>4.3</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="45" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="3">
+        <v>4</v>
+      </c>
+      <c r="E38" s="3">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B39" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C39" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="3">
-        <v>1</v>
-      </c>
-      <c r="E38" s="3">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="D39" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="3">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="45" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B40" s="1" t="s">
-        <v>104</v>
+        <v>46</v>
       </c>
       <c r="C40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D40" s="3">
+        <v>2</v>
+      </c>
+      <c r="E40" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B41" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D40" s="3">
-        <v>1</v>
-      </c>
-      <c r="E40" s="3">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B41" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="C41" s="3" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="D41" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E41" s="3">
         <v>4.5</v>
       </c>
     </row>
-    <row r="42" spans="2:5" ht="45" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
-        <v>83</v>
+        <v>47</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="3">
+        <v>2</v>
+      </c>
+      <c r="E42" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B43" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D42" s="3">
+      <c r="C43" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="3">
         <v>3</v>
-      </c>
-      <c r="E42" s="3">
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="3">
-        <v>1</v>
       </c>
       <c r="E43" s="3">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="45" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D44" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E44" s="3">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D45" s="3">
+        <v>2</v>
+      </c>
+      <c r="E45" s="3">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B46" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C46" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D45" s="3">
-        <v>1</v>
-      </c>
-      <c r="E45" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B46" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="D46" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" s="3">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B47" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D47" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E47" s="3">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="48" spans="2:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="B48" s="1" t="s">
+    <row r="48" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B48" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="3">
+        <v>3</v>
+      </c>
+      <c r="E48" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B49" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" s="3">
-        <v>1</v>
-      </c>
-      <c r="E48" s="3">
-        <v>6.2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="30" x14ac:dyDescent="0.15">
-      <c r="B49" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="C49" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D49" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" s="3">
         <v>6.2</v>
       </c>
     </row>
-    <row r="50" spans="2:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B50" s="1" t="s">
-        <v>62</v>
+        <v>106</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="D50" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E50" s="3">
         <v>6.2</v>
       </c>
     </row>
-    <row r="51" spans="2:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>84</v>
+        <v>61</v>
       </c>
       <c r="D51" s="3">
         <v>3</v>
       </c>
       <c r="E51" s="3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B52" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52" s="3">
+        <v>3</v>
+      </c>
+      <c r="E52" s="3">
         <v>6.3</v>
       </c>
     </row>
-    <row r="52" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B52" s="1" t="s">
+    <row r="53" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D52" s="3">
-        <v>1</v>
-      </c>
-      <c r="E52" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B53" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="C53" s="3" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="D53" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E53" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:5" ht="45" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>108</v>
+        <v>66</v>
       </c>
       <c r="D54" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E54" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="2:5" ht="30" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D55" s="3">
+        <v>3</v>
+      </c>
+      <c r="E55" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B56" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="C56" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D55" s="3">
-        <v>1</v>
-      </c>
-      <c r="E55" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="45" x14ac:dyDescent="0.15">
-      <c r="B56" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="D56" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E56" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="2:5" ht="45" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B57" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" s="3">
+        <v>2</v>
+      </c>
+      <c r="E57" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B58" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="C58" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D58" s="3">
         <v>3</v>
       </c>
-      <c r="E57" s="3">
+      <c r="E58" s="3">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first draft of acceptance tests
</commit_message>
<xml_diff>
--- a/doc/Model/Acceptance tests.xlsx
+++ b/doc/Model/Acceptance tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\sadna\Workshop-On-Software-Engineering-Project-2019\doc\Model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF89BF0-6FD7-4845-9E69-A444823816DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC7D37B6-63AC-4A2E-8680-D10B15A26E21}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1CA65076-1370-4905-AE0F-4695E8F49515}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
   <si>
     <t>data</t>
   </si>
@@ -65,9 +65,6 @@
     <t>המערכת תבקש מהמשתמש להכניס ערך בין 1 ל5 כפרמטר סינון</t>
   </si>
   <si>
-    <t>מה הוא טווח הדירוג? 1 - 5? 1- 10? כרגע הבדיקה מניחה 1 - 5</t>
-  </si>
-  <si>
     <t>מוצר אחד עם מזהה id_1 קיים בעגלת המשתמש</t>
   </si>
   <si>
@@ -92,48 +89,9 @@
     <t>2.8.1</t>
   </si>
   <si>
-    <t>המשתמש רוצה לקנות שני מוצרים -id_1, id_2-, אין סתירות במדיניות הרכישה וההנחות</t>
-  </si>
-  <si>
-    <t>הרכישה מופיעה בהיסטוריית הרכישה של המשתמש והחנות</t>
-  </si>
-  <si>
-    <t>המשתמש רוצה לקנות שני מוצרים -id_1, id_2-, יש סתירות במדיניות הרכישה ואין סתירה במדיניות וההנחות</t>
-  </si>
-  <si>
-    <t>המערכת מציגה הודעת שגיאה בה היא מפרטת שיש סתירה במידניות הרכישה. המוצרים אינם מופיעים באף הסטוריית רכישה</t>
-  </si>
-  <si>
     <t>2.8.2</t>
   </si>
   <si>
-    <t>פרטי משתמש שקיים במערכת, סכום לא שלילי לחיובי - 100$, למשתמש יש לפחות 100$ בחשבון שלו</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה אישור על כך שהגבייה התבצעה בהצלחה</t>
-  </si>
-  <si>
-    <t>פרטי משתמש שלא קיים במערכת, סכום לא שלילי לחיובי - 100$</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה שגיאה שמראה שהמשתמש לא קיים במערכת ושלא בוצעה גבייה</t>
-  </si>
-  <si>
-    <t>2.8.3</t>
-  </si>
-  <si>
-    <t>עסקה עליה יש אישור ממערכת הגבייה על כך שהעסקה התבצעה בהצלחה</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה אישור על כך שהתקבלה בקשת אספקה</t>
-  </si>
-  <si>
-    <t>עסקה עליה אין אישור ממערכת הגבייה על כך שהעסקה התבצעה בהצלחה</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה שגיאה שמראה על כך שבקשת האספקה נדחיתה</t>
-  </si>
-  <si>
     <t>המשתמש מחובר למערכת</t>
   </si>
   <si>
@@ -149,12 +107,6 @@
     <t>המוצר id_1 מוסר מהחנות</t>
   </si>
   <si>
-    <t>המשתמש אינו מזוהה כבעל החנות. הוא מסיר את המוצר id_1 אשר קיים בחנות</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על כך שעל מנת להסיר מוצר מהחנות חייב המשתמש להיות בעל החנות. המוצר id_1 עדיין קיים בחנות</t>
-  </si>
-  <si>
     <t>משתמש מזוהה כבעל חנות. והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי. יש ממנה יחיד לחנות</t>
   </si>
   <si>
@@ -227,12 +179,6 @@
     <t>המערכת מחזירה אישור כי העסקה בוצעה בהצלחה</t>
   </si>
   <si>
-    <t>המערכת מחזירה הודעת שגיאה על כך שיש סתירה בעסקה למדיניות החנות, ומודיעה שהעסקה לא התבצעה</t>
-  </si>
-  <si>
-    <t>המשתמש מבקש לבצע לרכוש מוצרים וקיימת סתירה למדיניות אותה הגדיר בעל החנות</t>
-  </si>
-  <si>
     <t>המערכת מחזירה אישור כי התקבלה הבקשה לאספקה וכן חוזר מספר משלוח</t>
   </si>
   <si>
@@ -260,9 +206,6 @@
     <t>המערכת מחזירה הודעת שגיאה על כך אחד פרטי המשתמש שגויים</t>
   </si>
   <si>
-    <t>המוצר אותו הזין המשתמש נמצא בתוצאות החיפוש</t>
-  </si>
-  <si>
     <t>בתוצאות החיפוש ישנם רק מוצרים מאותה קטגוריה</t>
   </si>
   <si>
@@ -275,18 +218,6 @@
     <t>המערכת מחזירה הודעה על כך שניתן להוסיף רק מנויים במערכת</t>
   </si>
   <si>
-    <t>משתמש מזוהה כבעל חנות ויש לו הרשאות רק להוריד ולהוסיף מוצרים. והמשתמש id_1 שאותו רוצים למנות מזוהה כמנוי.</t>
-  </si>
-  <si>
-    <t>המערכת מחזירה הודעה על זה שרק בעל החנות עם הרשאות להוסיף ולהסיר עובדים רשאי להסיר עובדים</t>
-  </si>
-  <si>
-    <t>משתמש אשר רשום כמנהל מערכת מסיר משתמש אשר קיים במערכת id_1 ומוגדר כבעל החנות עם חנויות id_2 ו id_3</t>
-  </si>
-  <si>
-    <t>המשתמש id_1 מוסר מהמערכת, וכן החנויות שלו id_2 וid_3 מוסרות מהמערכת</t>
-  </si>
-  <si>
     <t>משתמש id_1 מזוהה כבעל חנות אשר מונה על ידי משתמש id_2. המשתמש id_2 מנסה למנות לבעל החנות את Id_1</t>
   </si>
   <si>
@@ -305,9 +236,6 @@
     <t>המשתמש אורח, הוא מנסה להשתמש עם שם משתמש שקיים במערכת אך עם ססמא שגויה</t>
   </si>
   <si>
-    <t>חיפוש מוצר לפי מילות מפתח - 'candle'</t>
-  </si>
-  <si>
     <t>המערכת תציג למשתמש את כל המוצרים שהמילה candle מקושרת אליהם</t>
   </si>
   <si>
@@ -383,7 +311,73 @@
     <t>המערכת לא אותחלה והוצגה הודעת שגיאה</t>
   </si>
   <si>
-    <t>המשתמש מחפש מוצר לפי שם המוצר והמוצר קיים המערכת</t>
+    <t xml:space="preserve">המשתמש האורח רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום ופרטי אספקה </t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש האורח רוצה לקנות מוצר אחד Id_1 אשר לא קיים במערכת, מזין פרטי תשלום ופרטי אספקה </t>
+  </si>
+  <si>
+    <t>המערכת מודיעה כי לא קיים מוצר כמתואר והרכישה לא התבצעה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות בקנייה, מזין פרטי תשלום ופרטי אספקה </t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש האורח רוצה לקנות מספר מוצרים מעגלת הקניות כאשר לא כולם קיימים במערכת, מזין פרטי תשלום ופרטי אספקה </t>
+  </si>
+  <si>
+    <t>המערכת הציגה סכום לתשלום והרכישה התבצעה בהצלחה ומופיעה בהיסטוריית הרכישה של המשתמש והחנות</t>
+  </si>
+  <si>
+    <t>המערכת הציגה סכום לתשלום והמערכת מודיעה כי פרטי התשלום שגויים והרכישה לא התבצעה</t>
+  </si>
+  <si>
+    <t xml:space="preserve">המשתמש האורח רוצה לקנות מוצר אחד Id_1 אשר קיים במערכת, מזין פרטי תשלום עם אשראי לא תקינים ופרטי אספקה </t>
+  </si>
+  <si>
+    <t>חיפוש מוצר לפי שם מוצר - 'fur shampoo'</t>
+  </si>
+  <si>
+    <t>לא ממומש כרגע</t>
+  </si>
+  <si>
+    <t>4.1.1</t>
+  </si>
+  <si>
+    <t>4.1.2</t>
+  </si>
+  <si>
+    <t>4.1.3</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מוסיף את המוצר id_1 אשר לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>המוצר הוסף בהצלחה לחנות</t>
+  </si>
+  <si>
+    <t>המשתמש אינו מזוהה כבעל החנות. הוא מנסה להוסיף את המוצר id_1 אשר לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות</t>
+  </si>
+  <si>
+    <t>המוצר id_1 נערך בהצלחה</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שעל מנת להוסיף מוצר לחנות חייב המשתמש להיות בעל הרשאות. המוצר id_1 לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שעל מנת לערוך מוצר מהחנות חייב המשתמש להיות בעל הרשאות. המוצר id_1 נותר ללא שינוי</t>
+  </si>
+  <si>
+    <t>המשתמש מזוהה כבעל החנות. הוא מסיר את המוצר id_1 אשר לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>המערכת מחזירה הודעה על כך שהמוצר לא קיים בחנות</t>
+  </si>
+  <si>
+    <t>המשתמש אינו מזוהה כבעל החנות. הוא עורך את המוצר id_1 אשר קיים בחנות</t>
   </si>
 </sst>
 </file>
@@ -426,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -436,12 +430,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -788,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB44C02-4CA2-465F-A9FE-5F1D45ACF731}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -818,10 +806,10 @@
     </row>
     <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="D2" s="3">
         <v>1</v>
@@ -832,10 +820,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="D3" s="3">
         <v>2</v>
@@ -846,10 +834,10 @@
     </row>
     <row r="4" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="D4" s="3">
         <v>1</v>
@@ -860,10 +848,10 @@
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="D5" s="3">
         <v>2</v>
@@ -874,10 +862,10 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="D6" s="3">
         <v>3</v>
@@ -888,10 +876,10 @@
     </row>
     <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="3" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
@@ -902,10 +890,10 @@
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="D8" s="3">
         <v>2</v>
@@ -916,10 +904,10 @@
     </row>
     <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>90</v>
+        <v>67</v>
       </c>
       <c r="D9" s="3">
         <v>3</v>
@@ -930,10 +918,10 @@
     </row>
     <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
@@ -961,7 +949,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="D12" s="3">
         <v>3</v>
@@ -971,6 +959,9 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>102</v>
+      </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
@@ -986,7 +977,7 @@
     </row>
     <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>10</v>
@@ -1005,10 +996,10 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="D15" s="3">
         <v>6</v>
@@ -1018,23 +1009,21 @@
       </c>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="2"/>
+    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B16" s="3" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E16" s="3">
-        <v>2.5</v>
-      </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="58" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
         <v>12</v>
       </c>
@@ -1042,13 +1031,13 @@
         <v>15</v>
       </c>
       <c r="D17" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" s="3">
         <v>2.6</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="58" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
         <v>13</v>
       </c>
@@ -1056,35 +1045,35 @@
         <v>16</v>
       </c>
       <c r="D18" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E18" s="3">
         <v>2.6</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>17</v>
+        <v>70</v>
       </c>
       <c r="D19" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19" s="3">
-        <v>2.6</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B20" s="3" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="D20" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="3">
         <v>2.7</v>
@@ -1092,153 +1081,153 @@
     </row>
     <row r="21" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D21" s="3">
-        <v>2</v>
-      </c>
-      <c r="E21" s="3">
-        <v>2.7</v>
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="3" t="s">
-        <v>21</v>
+        <v>95</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>20</v>
+        <v>94</v>
       </c>
       <c r="D22" s="3">
-        <v>1</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>19</v>
+        <v>2</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>22</v>
+        <v>100</v>
       </c>
       <c r="D23" s="3">
-        <v>2</v>
-      </c>
-      <c r="E23" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B24" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>27</v>
+        <v>97</v>
       </c>
       <c r="D25" s="3">
         <v>2</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="E25" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B26" s="3" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="D26" s="3">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B27" s="3" t="s">
-        <v>33</v>
+        <v>3</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D27" s="3">
-        <v>2</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>29</v>
+        <v>1</v>
+      </c>
+      <c r="E27" s="3">
+        <v>3.1</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B28" s="1" t="s">
-        <v>35</v>
+      <c r="B28" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="D28" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28" s="3">
         <v>3.1</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B29" s="3" t="s">
-        <v>35</v>
+    <row r="29" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="D29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E29" s="3">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="D30" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E30" s="3">
         <v>3.2</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
       <c r="D31" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E31" s="3">
         <v>3.2</v>
@@ -1246,97 +1235,97 @@
     </row>
     <row r="32" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D32" s="3">
-        <v>3</v>
-      </c>
-      <c r="E32" s="3">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
-        <v>38</v>
+        <v>111</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>37</v>
+        <v>108</v>
       </c>
       <c r="D33" s="3">
-        <v>1</v>
-      </c>
-      <c r="E33" s="3">
-        <v>4.0999999999999996</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B34" s="3" t="s">
-        <v>40</v>
+        <v>2</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B34" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="D34" s="3">
-        <v>2</v>
-      </c>
-      <c r="E34" s="3">
-        <v>4.0999999999999996</v>
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B35" s="1" t="s">
-        <v>42</v>
+      <c r="B35" s="3" t="s">
+        <v>114</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="D35" s="3">
-        <v>1</v>
-      </c>
-      <c r="E35" s="3">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
-        <v>44</v>
+        <v>110</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>43</v>
+        <v>109</v>
       </c>
       <c r="D36" s="3">
-        <v>2</v>
-      </c>
-      <c r="E36" s="3">
-        <v>4.3</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B37" s="1" t="s">
-        <v>80</v>
+        <v>1</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B37" s="3" t="s">
+        <v>112</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="D37" s="3">
-        <v>3</v>
-      </c>
-      <c r="E37" s="3">
-        <v>4.3</v>
+        <v>2</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="D38" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E38" s="3">
         <v>4.3</v>
@@ -1344,181 +1333,181 @@
     </row>
     <row r="39" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D39" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="3">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="3">
+        <v>3</v>
+      </c>
+      <c r="E40" s="3">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B41" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="3">
+        <v>4</v>
+      </c>
+      <c r="E41" s="3">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B42" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3">
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B40" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="3">
-        <v>2</v>
-      </c>
-      <c r="E40" s="3">
+    <row r="43" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B43" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="3">
+        <v>2</v>
+      </c>
+      <c r="E43" s="3">
         <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B41" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D41" s="3">
-        <v>1</v>
-      </c>
-      <c r="E41" s="3">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B42" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D42" s="3">
-        <v>2</v>
-      </c>
-      <c r="E42" s="3">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B43" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="3">
-        <v>3</v>
-      </c>
-      <c r="E43" s="3">
-        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="D44" s="3">
         <v>1</v>
       </c>
       <c r="E44" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B45" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="3">
+        <v>2</v>
+      </c>
+      <c r="E45" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B46" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="3">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="45" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B45" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D45" s="3">
-        <v>2</v>
-      </c>
-      <c r="E45" s="3">
+    <row r="47" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B47" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D47" s="3">
+        <v>2</v>
+      </c>
+      <c r="E47" s="3">
         <v>4.5999999999999996</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B46" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D46" s="3">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B47" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D47" s="3">
-        <v>2</v>
-      </c>
-      <c r="E47" s="3">
-        <v>5.0999999999999996</v>
-      </c>
-    </row>
     <row r="48" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B48" s="3" t="s">
-        <v>58</v>
+      <c r="B48" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D48" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E48" s="3">
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="49" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B49" s="1" t="s">
-        <v>60</v>
+    <row r="49" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B49" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>104</v>
+        <v>40</v>
       </c>
       <c r="D49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E49" s="3">
-        <v>6.2</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="50" spans="2:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="B50" s="1" t="s">
-        <v>106</v>
+      <c r="B50" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>105</v>
+        <v>41</v>
       </c>
       <c r="D50" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E50" s="3">
-        <v>6.2</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="51" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B51" s="1" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D51" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E51" s="3">
         <v>6.2</v>
@@ -1526,41 +1515,41 @@
     </row>
     <row r="52" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B52" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D52" s="3">
+        <v>2</v>
+      </c>
+      <c r="E52" s="3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="B53" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" s="3">
         <v>3</v>
       </c>
-      <c r="E52" s="3">
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D53" s="3">
-        <v>1</v>
-      </c>
       <c r="E53" s="3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B54" s="1" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="D54" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" s="3">
         <v>7</v>
@@ -1568,13 +1557,13 @@
     </row>
     <row r="55" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B55" s="1" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="D55" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E55" s="3">
         <v>7</v>
@@ -1582,10 +1571,10 @@
     </row>
     <row r="56" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B56" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D56" s="3">
         <v>1</v>
@@ -1596,10 +1585,10 @@
     </row>
     <row r="57" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B57" s="1" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="D57" s="3">
         <v>2</v>
@@ -1610,10 +1599,10 @@
     </row>
     <row r="58" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B58" s="1" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="D58" s="3">
         <v>3</v>

</xml_diff>